<commit_message>
Actualización de la documentación y contratos
</commit_message>
<xml_diff>
--- a/Documentación/Empresa/Control de equipos.xlsx
+++ b/Documentación/Empresa/Control de equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\GitHub\dta-agricola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L03502024\Documents\GitHub\dta-agricola\Documentación\Empresa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE7B99D-04E6-488C-8428-BE1B6CF6D7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23581048-E9DE-4345-9FD1-B1799B4A2BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="458" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="458" xr2:uid="{81E9D037-BE23-435E-B775-5A4C621A153A}"/>
   </bookViews>
   <sheets>
     <sheet name="Movimiento contínuo" sheetId="8" r:id="rId1"/>
@@ -633,288 +633,236 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1233,49 +1181,49 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="15" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="15" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="19.140625" style="15" customWidth="1"/>
-    <col min="18" max="18" width="60.28515625" style="20" customWidth="1"/>
-    <col min="19" max="26" width="12.140625" style="17" customWidth="1"/>
-    <col min="27" max="16384" width="11.5703125" style="15"/>
+    <col min="1" max="1" width="5.1796875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="12" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="31.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="19.1796875" style="12" customWidth="1"/>
+    <col min="18" max="18" width="60.26953125" style="15" customWidth="1"/>
+    <col min="19" max="26" width="12.1796875" style="13" customWidth="1"/>
+    <col min="27" max="16384" width="11.54296875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="R1" s="66" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="R1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-    </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+    </row>
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1309,25 +1257,25 @@
       <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="2" t="s">
         <v>46</v>
       </c>
       <c r="S2" s="1">
@@ -1355,1172 +1303,1161 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>526251106286</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="6">
         <v>1211</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="8" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="9">
         <v>43872</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-    </row>
-    <row r="4" spans="1:26" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="22">
         <v>526251271378</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="23">
         <v>1211</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31" t="s">
+      <c r="H4" s="23"/>
+      <c r="I4" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="28" t="s">
+      <c r="N4" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O4" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="P4" s="35">
+      <c r="P4" s="26">
         <v>44603</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="R4" s="36" t="s">
+      <c r="R4" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-    </row>
-    <row r="5" spans="1:26" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+    </row>
+    <row r="5" spans="1:26" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="22">
         <v>526251024489</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="23">
         <v>1211</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31" t="s">
+      <c r="H5" s="23"/>
+      <c r="I5" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="N5" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="34" t="s">
+      <c r="O5" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="P5" s="35">
+      <c r="P5" s="26">
         <v>44603</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="Q5" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="R5" s="36" t="s">
+      <c r="R5" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="32"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="32"/>
-    </row>
-    <row r="6" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+    </row>
+    <row r="6" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="20">
         <v>4</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="22">
         <v>526251452797</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="23">
         <v>1211</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31" t="s">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="28" t="s">
+      <c r="N6" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="34" t="s">
+      <c r="O6" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="P6" s="35">
+      <c r="P6" s="26">
         <v>44603</v>
       </c>
-      <c r="Q6" s="28" t="s">
+      <c r="Q6" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="36" t="s">
+      <c r="R6" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
-    </row>
-    <row r="7" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+    </row>
+    <row r="7" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20">
         <v>5</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="22">
         <v>526255917395</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="23">
         <v>1211</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31" t="s">
+      <c r="H7" s="23"/>
+      <c r="I7" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K7" s="33" t="s">
+      <c r="K7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="28" t="s">
+      <c r="N7" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="O7" s="34" t="s">
+      <c r="O7" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="P7" s="35">
+      <c r="P7" s="26">
         <v>44603</v>
       </c>
-      <c r="Q7" s="28" t="s">
+      <c r="Q7" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="R7" s="36" t="s">
+      <c r="R7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="32"/>
-    </row>
-    <row r="8" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+    </row>
+    <row r="8" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20">
         <v>6</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="22">
         <v>526251193016</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="23">
         <v>1211</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="28" t="s">
+      <c r="L8" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="28" t="s">
+      <c r="M8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="28" t="s">
+      <c r="N8" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="P8" s="35">
+      <c r="P8" s="26">
         <v>44603</v>
       </c>
-      <c r="Q8" s="28" t="s">
+      <c r="Q8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="R8" s="36" t="s">
+      <c r="R8" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="32"/>
-      <c r="Y8" s="32"/>
-      <c r="Z8" s="32"/>
-    </row>
-    <row r="9" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+    </row>
+    <row r="9" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20">
         <v>7</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="22">
         <v>526251342314</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="23">
         <v>1211</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="N9" s="28" t="s">
+      <c r="N9" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="O9" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="P9" s="35">
+      <c r="P9" s="26">
         <v>44603</v>
       </c>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="R9" s="36" t="s">
+      <c r="R9" s="27" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57">
+    <row r="10" spans="1:26" s="45" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="45">
         <v>8</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="59">
+      <c r="C10" s="47">
         <v>526251201079</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="61" t="s">
+      <c r="E10" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="61" t="s">
+      <c r="F10" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="61">
+      <c r="G10" s="48">
         <v>1211</v>
       </c>
-      <c r="H10" s="61" t="s">
+      <c r="H10" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="K10" s="62" t="s">
+      <c r="K10" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="57" t="s">
+      <c r="L10" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="57" t="s">
+      <c r="M10" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="O10" s="63" t="s">
+      <c r="O10" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="P10" s="64">
+      <c r="P10" s="51">
         <v>44384</v>
       </c>
-      <c r="Q10" s="57" t="s">
+      <c r="Q10" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="R10" s="65" t="s">
+      <c r="R10" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="S10" s="61"/>
-      <c r="T10" s="61"/>
-      <c r="U10" s="61"/>
-      <c r="V10" s="61"/>
-      <c r="W10" s="61"/>
-      <c r="X10" s="61"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="61"/>
-    </row>
-    <row r="11" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="48"/>
+    </row>
+    <row r="11" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="29">
         <v>9</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="31">
         <v>526251020232</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="32">
         <v>1312</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="I11" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="44" t="s">
+      <c r="J11" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="K11" s="45" t="s">
+      <c r="K11" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="46" t="s">
+      <c r="L11" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="46" t="s">
+      <c r="M11" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="46" t="s">
+      <c r="N11" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="O11" s="47" t="s">
+      <c r="O11" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="P11" s="47">
+      <c r="P11" s="35">
         <v>44646</v>
       </c>
-      <c r="R11" s="48"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-    </row>
-    <row r="12" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="R11" s="36"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="32"/>
+    </row>
+    <row r="12" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="29">
         <v>10</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="37">
         <v>526251531996</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="32">
         <v>1211</v>
       </c>
-      <c r="H12" s="42" t="s">
+      <c r="H12" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I12" s="42" t="s">
+      <c r="I12" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="J12" s="44" t="s">
+      <c r="J12" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="K12" s="45" t="s">
+      <c r="K12" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="46" t="s">
+      <c r="L12" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="M12" s="46" t="s">
+      <c r="M12" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="N12" s="46" t="s">
+      <c r="N12" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="O12" s="50" t="s">
+      <c r="O12" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="P12" s="47">
+      <c r="P12" s="35">
         <v>44646</v>
       </c>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="51" t="s">
+      <c r="Q12" s="34"/>
+      <c r="R12" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="S12" s="43" t="s">
+      <c r="S12" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="T12" s="43" t="s">
+      <c r="T12" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="U12" s="43" t="s">
+      <c r="U12" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="V12" s="43" t="s">
+      <c r="V12" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="W12" s="43" t="s">
+      <c r="W12" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="X12" s="43" t="s">
+      <c r="X12" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="Y12" s="52" t="s">
+      <c r="Y12" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="Z12" s="43" t="s">
+      <c r="Z12" s="32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39">
+    <row r="13" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="29">
         <v>11</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="37">
         <v>526258372598</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="42">
+      <c r="G13" s="32">
         <v>1211</v>
       </c>
-      <c r="H13" s="42" t="s">
+      <c r="H13" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I13" s="42" t="s">
+      <c r="I13" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="J13" s="44" t="s">
+      <c r="J13" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="K13" s="45" t="s">
+      <c r="K13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="46" t="s">
+      <c r="L13" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="46" t="s">
+      <c r="M13" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="N13" s="46" t="s">
+      <c r="N13" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="O13" s="50" t="s">
+      <c r="O13" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="P13" s="47">
+      <c r="P13" s="35">
         <v>44646</v>
       </c>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="43"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="43"/>
-      <c r="Z13" s="43"/>
-    </row>
-    <row r="14" spans="1:26" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="Q13" s="34"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="32"/>
+    </row>
+    <row r="14" spans="1:26" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="29">
         <v>12</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="37">
         <v>526251259145</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="G14" s="42">
+      <c r="G14" s="32">
         <v>1211</v>
       </c>
-      <c r="H14" s="42" t="s">
+      <c r="H14" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I14" s="42" t="s">
+      <c r="I14" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="J14" s="44" t="s">
+      <c r="J14" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="K14" s="45" t="s">
+      <c r="K14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="46" t="s">
+      <c r="L14" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="M14" s="46" t="s">
+      <c r="M14" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="N14" s="46" t="s">
+      <c r="N14" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="O14" s="47" t="s">
+      <c r="O14" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="P14" s="47">
+      <c r="P14" s="35">
         <v>44646</v>
       </c>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="54" t="s">
+      <c r="Q14" s="34"/>
+      <c r="R14" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="S14" s="55" t="s">
+      <c r="S14" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="T14" s="43" t="s">
+      <c r="T14" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="U14" s="43" t="s">
+      <c r="U14" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="V14" s="43" t="s">
+      <c r="V14" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="W14" s="43" t="s">
+      <c r="W14" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="X14" s="43" t="s">
+      <c r="X14" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="Y14" s="43" t="s">
+      <c r="Y14" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="Z14" s="43" t="s">
+      <c r="Z14" s="32" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39">
+    <row r="15" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="29">
         <v>13</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="37">
         <v>526251037317</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="42">
+      <c r="G15" s="32">
         <v>1312</v>
       </c>
-      <c r="H15" s="42" t="s">
+      <c r="H15" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="42" t="s">
+      <c r="I15" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="K15" s="45" t="s">
+      <c r="K15" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="46" t="s">
+      <c r="L15" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="46" t="s">
+      <c r="M15" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="N15" s="46" t="s">
+      <c r="N15" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="50" t="s">
+      <c r="O15" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="P15" s="47">
+      <c r="P15" s="35">
         <v>44646</v>
       </c>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="56" t="s">
+      <c r="Q15" s="34"/>
+      <c r="R15" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="S15" s="43"/>
-      <c r="T15" s="43"/>
-      <c r="U15" s="43"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="43"/>
-      <c r="X15" s="43"/>
-      <c r="Y15" s="43"/>
-      <c r="Z15" s="43"/>
-    </row>
-    <row r="16" spans="1:26" s="39" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39">
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="32"/>
+      <c r="Z15" s="32"/>
+    </row>
+    <row r="16" spans="1:26" s="29" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="29">
         <v>14</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="37">
         <v>526251060168</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="G16" s="42">
+      <c r="G16" s="32">
         <v>1211</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="J16" s="44" t="s">
+      <c r="J16" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="K16" s="45" t="s">
+      <c r="K16" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L16" s="46" t="s">
+      <c r="L16" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="M16" s="39" t="s">
+      <c r="M16" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="N16" s="39" t="s">
+      <c r="N16" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="O16" s="50" t="s">
+      <c r="O16" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="P16" s="47">
+      <c r="P16" s="35">
         <v>44762</v>
       </c>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="51" t="s">
+      <c r="Q16" s="34"/>
+      <c r="R16" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
-      <c r="U16" s="43"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="43"/>
-      <c r="X16" s="43"/>
-      <c r="Y16" s="43"/>
-      <c r="Z16" s="43"/>
-    </row>
-    <row r="17" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="32"/>
+    </row>
+    <row r="17" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="20">
         <v>15</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="22">
         <v>526251059200</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="23">
         <v>1211</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31" t="s">
+      <c r="H17" s="23"/>
+      <c r="I17" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="33" t="s">
+      <c r="K17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L17" s="67" t="s">
+      <c r="L17" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="M17" s="67" t="s">
+      <c r="M17" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="67" t="s">
+      <c r="N17" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="O17" s="68" t="s">
+      <c r="O17" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="P17" s="34">
+      <c r="P17" s="25">
         <v>44647</v>
       </c>
-      <c r="Q17" s="67"/>
-      <c r="R17" s="69"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="32"/>
-    </row>
-    <row r="18" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
+      <c r="Q17" s="24"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
+    </row>
+    <row r="18" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="20">
         <v>16</v>
       </c>
-      <c r="B18" s="89" t="s">
+      <c r="B18" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="70">
+      <c r="C18" s="55">
         <v>526251020790</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="23">
         <v>1211</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="31" t="s">
+      <c r="H18" s="23"/>
+      <c r="I18" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="33" t="s">
+      <c r="K18" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="67" t="s">
+      <c r="L18" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="M18" s="67" t="s">
+      <c r="M18" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="N18" s="67" t="s">
+      <c r="N18" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="O18" s="68" t="s">
+      <c r="O18" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="P18" s="34">
+      <c r="P18" s="25">
         <v>44647</v>
       </c>
-      <c r="R18" s="69"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="32"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="32"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="24">
+      <c r="R18" s="54"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A19" s="17">
         <v>17</v>
       </c>
-      <c r="B19" s="90" t="s">
+      <c r="B19" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="18">
         <v>526251020642</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="13">
         <v>1211</v>
       </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="16" t="s">
+      <c r="H19" s="13"/>
+      <c r="I19" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A20" s="12">
         <v>18</v>
       </c>
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="18">
         <v>526251020596</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="95">
+      <c r="G20" s="13">
         <v>1211</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="16" t="s">
+      <c r="H20" s="13"/>
+      <c r="I20" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A21" s="12">
         <v>19</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="71">
+      <c r="C21" s="56">
         <v>526251579804</v>
       </c>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="72">
+      <c r="G21" s="13">
         <v>1211</v>
       </c>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72" t="s">
+      <c r="H21" s="13"/>
+      <c r="I21" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K21" s="73" t="s">
+      <c r="K21" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O21" s="74"/>
-      <c r="P21" s="75"/>
-      <c r="R21" s="76"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-    </row>
-    <row r="23" spans="1:26" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="81" t="s">
+      <c r="O21" s="57"/>
+      <c r="P21" s="58"/>
+      <c r="R21" s="59"/>
+    </row>
+    <row r="23" spans="1:26" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="D23" s="81" t="s">
+      <c r="D23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="81" t="s">
+      <c r="E23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="F23" s="81" t="s">
+      <c r="F23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="81" t="s">
+      <c r="G23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="H23" s="81" t="s">
+      <c r="H23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="I23" s="81" t="s">
+      <c r="I23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="J23" s="81" t="s">
+      <c r="J23" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="K23" s="78" t="s">
+      <c r="K23" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="77" t="s">
+      <c r="L23" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="M23" s="79" t="s">
+      <c r="M23" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="N23" s="77" t="s">
+      <c r="N23" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="O23" s="94" t="s">
+      <c r="O23" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="R23" s="80"/>
-      <c r="S23" s="81"/>
-      <c r="T23" s="81"/>
-      <c r="U23" s="81"/>
-      <c r="V23" s="81"/>
-      <c r="W23" s="81"/>
-      <c r="X23" s="81"/>
-      <c r="Y23" s="81"/>
-      <c r="Z23" s="81"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="64"/>
+      <c r="T23" s="64"/>
+      <c r="U23" s="64"/>
+      <c r="V23" s="64"/>
+      <c r="W23" s="64"/>
+      <c r="X23" s="64"/>
+      <c r="Y23" s="64"/>
+      <c r="Z23" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2534,40 +2471,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F66C39-03D2-4899-ADCF-3C8A8410502E}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="15" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="15" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="33.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="19.140625" style="15" customWidth="1"/>
-    <col min="18" max="18" width="60.28515625" style="20" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="15"/>
+    <col min="1" max="1" width="5.1796875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="12" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="33.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="19.1796875" style="12" customWidth="1"/>
+    <col min="18" max="18" width="60.26953125" style="15" customWidth="1"/>
+    <col min="19" max="16384" width="11.54296875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R1" s="38" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2601,82 +2538,79 @@
       <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="38" t="s">
+      <c r="R2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28">
+    <row r="3" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="O3" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="P3" s="35">
+      <c r="P3" s="26">
         <v>44603</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="36" t="s">
+      <c r="R3" s="27" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2691,332 +2625,330 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="83" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="83" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="83"/>
-    <col min="5" max="5" width="36.85546875" style="83" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="83"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="69" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="69" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="91">
+      <c r="B2" s="73">
         <v>526251106286</v>
       </c>
-      <c r="C2" s="82">
+      <c r="C2" s="65">
         <v>32845128</v>
       </c>
-      <c r="D2" s="82">
+      <c r="D2" s="65">
         <v>18</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="85" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="92">
+      <c r="B3" s="74">
         <v>526251024489</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="68">
         <v>32845129</v>
       </c>
-      <c r="D3" s="86">
+      <c r="D3" s="68">
         <v>18</v>
       </c>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="73">
         <v>526251531996</v>
       </c>
-      <c r="C4" s="82">
+      <c r="C4" s="65">
         <v>32845130</v>
       </c>
-      <c r="D4" s="82">
+      <c r="D4" s="65">
         <v>18</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="85" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="92">
+      <c r="B5" s="74">
         <v>526258372598</v>
       </c>
-      <c r="C5" s="86">
+      <c r="C5" s="68">
         <v>32845131</v>
       </c>
-      <c r="D5" s="86">
+      <c r="D5" s="68">
         <v>18</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="84" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="91">
+      <c r="B6" s="73">
         <v>526251059200</v>
       </c>
-      <c r="C6" s="82">
+      <c r="C6" s="65">
         <v>32845132</v>
       </c>
-      <c r="D6" s="82">
+      <c r="D6" s="65">
         <v>18</v>
       </c>
-      <c r="E6" s="82" t="s">
+      <c r="E6" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="85" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="92">
+      <c r="B7" s="74">
         <v>526251259145</v>
       </c>
-      <c r="C7" s="86">
+      <c r="C7" s="68">
         <v>32845134</v>
       </c>
-      <c r="D7" s="86">
+      <c r="D7" s="68">
         <v>18</v>
       </c>
-      <c r="E7" s="86" t="s">
+      <c r="E7" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="84" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="91">
+      <c r="B8" s="73">
         <v>526255917395</v>
       </c>
-      <c r="C8" s="82">
+      <c r="C8" s="65">
         <v>32845135</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="65">
         <v>18</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="85" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="92">
+      <c r="B9" s="74">
         <v>526251271378</v>
       </c>
-      <c r="C9" s="86">
+      <c r="C9" s="68">
         <v>32848029</v>
       </c>
-      <c r="D9" s="86">
+      <c r="D9" s="68">
         <v>18</v>
       </c>
-      <c r="E9" s="86" t="s">
+      <c r="E9" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="84" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="91">
+      <c r="B10" s="73">
         <v>526251193016</v>
       </c>
-      <c r="C10" s="82">
+      <c r="C10" s="65">
         <v>32848031</v>
       </c>
-      <c r="D10" s="82">
+      <c r="D10" s="65">
         <v>18</v>
       </c>
-      <c r="E10" s="82" t="s">
+      <c r="E10" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="85" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="92">
+      <c r="B11" s="74">
         <v>526251060168</v>
       </c>
-      <c r="C11" s="86">
+      <c r="C11" s="68">
         <v>32848045</v>
       </c>
-      <c r="D11" s="86">
+      <c r="D11" s="68">
         <v>18</v>
       </c>
-      <c r="E11" s="86" t="s">
+      <c r="E11" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="84" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="91">
+      <c r="B12" s="73">
         <v>526251037317</v>
       </c>
-      <c r="C12" s="82">
+      <c r="C12" s="65">
         <v>32848094</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="65">
         <v>32</v>
       </c>
-      <c r="E12" s="82" t="s">
+      <c r="E12" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="85" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="92">
+      <c r="B13" s="74">
         <v>526251452797</v>
       </c>
-      <c r="C13" s="86">
+      <c r="C13" s="68">
         <v>32848096</v>
       </c>
-      <c r="D13" s="86">
+      <c r="D13" s="68">
         <v>32</v>
       </c>
-      <c r="E13" s="86" t="s">
+      <c r="E13" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="84" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="91">
+      <c r="B14" s="73">
         <v>526251342314</v>
       </c>
-      <c r="C14" s="82">
+      <c r="C14" s="65">
         <v>32848097</v>
       </c>
-      <c r="D14" s="82">
+      <c r="D14" s="65">
         <v>32</v>
       </c>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="85" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="92">
+      <c r="B15" s="74">
         <v>526251579804</v>
       </c>
-      <c r="C15" s="86">
+      <c r="C15" s="68">
         <v>32848098</v>
       </c>
-      <c r="D15" s="86">
+      <c r="D15" s="68">
         <v>32</v>
       </c>
-      <c r="E15" s="86" t="s">
+      <c r="E15" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="84" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="91">
+      <c r="B16" s="73">
         <v>526251201079</v>
       </c>
-      <c r="C16" s="82">
+      <c r="C16" s="65">
         <v>32848099</v>
       </c>
-      <c r="D16" s="82">
+      <c r="D16" s="65">
         <v>32</v>
       </c>
-      <c r="E16" s="82" t="s">
+      <c r="E16" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="93" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="92">
+      <c r="B18" s="74">
         <v>526251020232</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="86" t="s">
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="83" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="91">
+      <c r="B19" s="73">
         <v>526251020790</v>
       </c>
-      <c r="E19" s="82" t="s">
+      <c r="E19" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="93" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="92">
+      <c r="B20" s="74">
         <v>526251020642</v>
       </c>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="86" t="s">
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="83" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="91">
+      <c r="B21" s="73">
         <v>526251020596</v>
       </c>
-      <c r="E21" s="82" t="s">
+      <c r="E21" s="65" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizaciones de SW y HW
HW:
- Se recuperó el proyecto de Pv66
Embebido:
- Se está trabajando en mejoras sobre el control de actuadores
- Bug en teléfonos con últimos dígitos mejor que 999.
</commit_message>
<xml_diff>
--- a/Documentación/Empresa/Control de equipos.xlsx
+++ b/Documentación/Empresa/Control de equipos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L03502024\Documents\GitHub\dta-agricola\Documentación\Empresa\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAB3C8C-3475-4638-88B9-9C4EFD788FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" tabRatio="458"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="458" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movimiento contínuo" sheetId="8" r:id="rId1"/>
@@ -237,9 +243,6 @@
     <t>3 2</t>
   </si>
   <si>
-    <t>{0, 3, 2, 12, 11, 1, 52, 625, 1201079}</t>
-  </si>
-  <si>
     <t>Pv66 v0.2.4.220529 A</t>
   </si>
   <si>
@@ -505,19 +508,16 @@
   </si>
   <si>
     <t>ECHEMENDIA NARANJO MIRIAM ESTHER</t>
+  </si>
+  <si>
+    <t>{0, 3, 2, 12, 11, 0, 52, 625, 1201079}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="28">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,7 +554,6 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -584,151 +583,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="41">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -737,19 +593,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.349986266670736"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149998474074526"/>
+        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,7 +617,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,198 +635,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -987,253 +657,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1263,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1287,41 +718,29 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1332,9 +751,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1371,9 +787,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1410,9 +823,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1422,10 +832,10 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1434,19 +844,16 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1455,11 +862,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1473,10 +877,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1488,7 +892,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1497,13 +901,10 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1518,7 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1527,65 +928,25 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
-    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
-    <cellStyle name="Coma" xfId="6" builtinId="3"/>
-    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21"/>
-    <cellStyle name="Nota" xfId="11" builtinId="10"/>
-    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
-    <cellStyle name="Título" xfId="14" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
-    <cellStyle name="Total" xfId="22" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
-    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
-    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
-    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
-    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
-    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1843,59 +1204,58 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="$A14:$XFD14"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5428571428571" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.18095238095238" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.4571428571429" style="12" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" style="12" customWidth="1"/>
     <col min="3" max="3" width="17" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.1809523809524" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="12" customWidth="1"/>
     <col min="5" max="5" width="10" style="12" customWidth="1"/>
-    <col min="6" max="6" width="6.81904761904762" style="12" customWidth="1"/>
-    <col min="7" max="7" width="7.54285714285714" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.45714285714286" style="12" customWidth="1"/>
-    <col min="9" max="9" width="31.2666666666667" style="12" customWidth="1"/>
-    <col min="10" max="10" width="19.4571428571429" style="12" customWidth="1"/>
-    <col min="11" max="11" width="37.8190476190476" style="12" customWidth="1"/>
-    <col min="12" max="12" width="15.4571428571429" style="12" customWidth="1"/>
-    <col min="13" max="13" width="20.2666666666667" style="12" customWidth="1"/>
-    <col min="14" max="14" width="10.8190476190476" style="12" customWidth="1"/>
-    <col min="15" max="15" width="26.1809523809524" style="12" customWidth="1"/>
-    <col min="16" max="17" width="19.1809523809524" style="12" customWidth="1"/>
-    <col min="18" max="18" width="60.2666666666667" style="13" customWidth="1"/>
-    <col min="19" max="26" width="12.1809523809524" style="36" customWidth="1"/>
-    <col min="27" max="16384" width="11.5428571428571" style="12"/>
+    <col min="6" max="6" width="6.81640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="31.26953125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="37.81640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="20.26953125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="26.1796875" style="12" customWidth="1"/>
+    <col min="16" max="17" width="19.1796875" style="12" customWidth="1"/>
+    <col min="18" max="18" width="60.26953125" style="13" customWidth="1"/>
+    <col min="19" max="26" width="12.1796875" style="31" customWidth="1"/>
+    <col min="27" max="16384" width="11.54296875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="18:26">
-      <c r="R1" s="14" t="s">
+    <row r="1" spans="1:26">
+      <c r="R1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-    </row>
-    <row r="2" s="9" customFormat="1" spans="1:26">
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="90"/>
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+    </row>
+    <row r="2" spans="1:26" s="9" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1975,55 +1335,55 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" s="30" customFormat="1" spans="1:26">
-      <c r="A3" s="37">
+    <row r="3" spans="1:26" s="11" customFormat="1">
+      <c r="A3" s="32">
         <v>1</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="34">
         <v>526251106286</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="35">
         <v>1211</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="40" t="s">
+      <c r="H3" s="35"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="64" t="s">
+      <c r="O3" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="65">
+      <c r="P3" s="58">
         <v>43872</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="Q3" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="85" t="s">
+      <c r="R3" s="76" t="s">
         <v>29</v>
       </c>
       <c r="S3" s="9"/>
@@ -2035,7 +1395,7 @@
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
     </row>
-    <row r="4" s="10" customFormat="1" ht="30" spans="1:26">
+    <row r="4" spans="1:26" s="10" customFormat="1" ht="29">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -2064,7 +1424,7 @@
       <c r="J4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="66" t="s">
+      <c r="K4" s="59" t="s">
         <v>23</v>
       </c>
       <c r="L4" s="10" t="s">
@@ -2076,16 +1436,16 @@
       <c r="N4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="26">
+      <c r="P4" s="24">
         <v>44603</v>
       </c>
       <c r="Q4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="27" t="s">
+      <c r="R4" s="25" t="s">
         <v>38</v>
       </c>
       <c r="S4" s="17"/>
@@ -2097,7 +1457,7 @@
       <c r="Y4" s="17"/>
       <c r="Z4" s="17"/>
     </row>
-    <row r="5" s="10" customFormat="1" ht="30" spans="1:26">
+    <row r="5" spans="1:26" s="10" customFormat="1" ht="29">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -2126,7 +1486,7 @@
       <c r="J5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="66" t="s">
+      <c r="K5" s="59" t="s">
         <v>23</v>
       </c>
       <c r="L5" s="10" t="s">
@@ -2138,16 +1498,16 @@
       <c r="N5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="24" t="s">
+      <c r="O5" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="P5" s="26">
+      <c r="P5" s="24">
         <v>44603</v>
       </c>
       <c r="Q5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="27" t="s">
+      <c r="R5" s="25" t="s">
         <v>38</v>
       </c>
       <c r="S5" s="17"/>
@@ -2159,7 +1519,7 @@
       <c r="Y5" s="17"/>
       <c r="Z5" s="17"/>
     </row>
-    <row r="6" s="10" customFormat="1" spans="1:26">
+    <row r="6" spans="1:26" s="10" customFormat="1">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -2188,7 +1548,7 @@
       <c r="J6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="66" t="s">
+      <c r="K6" s="59" t="s">
         <v>23</v>
       </c>
       <c r="L6" s="10" t="s">
@@ -2200,16 +1560,16 @@
       <c r="N6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="O6" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="P6" s="26">
+      <c r="P6" s="24">
         <v>44603</v>
       </c>
       <c r="Q6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="27" t="s">
+      <c r="R6" s="25" t="s">
         <v>49</v>
       </c>
       <c r="S6" s="17"/>
@@ -2221,7 +1581,7 @@
       <c r="Y6" s="17"/>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" s="10" customFormat="1" spans="1:26">
+    <row r="7" spans="1:26" s="10" customFormat="1">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -2250,7 +1610,7 @@
       <c r="J7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="66" t="s">
+      <c r="K7" s="59" t="s">
         <v>23</v>
       </c>
       <c r="L7" s="10" t="s">
@@ -2262,16 +1622,16 @@
       <c r="N7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="24">
         <v>44603</v>
       </c>
       <c r="Q7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R7" s="27" t="s">
+      <c r="R7" s="25" t="s">
         <v>49</v>
       </c>
       <c r="S7" s="17"/>
@@ -2283,7 +1643,7 @@
       <c r="Y7" s="17"/>
       <c r="Z7" s="17"/>
     </row>
-    <row r="8" s="10" customFormat="1" spans="1:26">
+    <row r="8" spans="1:26" s="10" customFormat="1">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -2312,7 +1672,7 @@
       <c r="J8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="66" t="s">
+      <c r="K8" s="59" t="s">
         <v>23</v>
       </c>
       <c r="L8" s="10" t="s">
@@ -2324,16 +1684,16 @@
       <c r="N8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="O8" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="24">
         <v>44603</v>
       </c>
       <c r="Q8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="27" t="s">
+      <c r="R8" s="25" t="s">
         <v>49</v>
       </c>
       <c r="S8" s="17"/>
@@ -2345,7 +1705,7 @@
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
     </row>
-    <row r="9" s="10" customFormat="1" spans="1:18">
+    <row r="9" spans="1:26" s="10" customFormat="1">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -2376,7 +1736,7 @@
       <c r="J9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="66" t="s">
+      <c r="K9" s="59" t="s">
         <v>23</v>
       </c>
       <c r="L9" s="10" t="s">
@@ -2388,494 +1748,494 @@
       <c r="N9" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="O9" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="P9" s="26">
+      <c r="P9" s="24">
         <v>44603</v>
       </c>
       <c r="Q9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R9" s="27" t="s">
+      <c r="R9" s="25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" s="31" customFormat="1" spans="1:26">
-      <c r="A10" s="31">
+    <row r="10" spans="1:26" s="27" customFormat="1">
+      <c r="A10" s="27">
         <v>8</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="37">
         <v>526251201079</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="38">
         <v>1211</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="J10" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="43" t="s">
+      <c r="K10" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="67" t="s">
+      <c r="M10" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="P10" s="62">
+        <v>44384</v>
+      </c>
+      <c r="Q10" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+    </row>
+    <row r="11" spans="1:26" s="28" customFormat="1">
+      <c r="A11" s="28">
+        <v>9</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="40">
+        <v>526251020232</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="41">
+        <v>1312</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="O10" s="68" t="s">
-        <v>77</v>
-      </c>
-      <c r="P10" s="69">
-        <v>44384</v>
-      </c>
-      <c r="Q10" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="43"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="43"/>
-      <c r="X10" s="43"/>
-      <c r="Y10" s="43"/>
-      <c r="Z10" s="43"/>
-    </row>
-    <row r="11" s="32" customFormat="1" spans="1:26">
-      <c r="A11" s="32">
-        <v>9</v>
-      </c>
-      <c r="B11" s="44" t="s">
+      <c r="L11" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="M11" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="N11" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="O11" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="P11" s="64">
+        <v>44646</v>
+      </c>
+      <c r="R11" s="78"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+    </row>
+    <row r="12" spans="1:26" s="29" customFormat="1">
+      <c r="A12" s="29">
+        <v>10</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="43">
+        <v>526251531996</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="44">
+        <v>1211</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="N12" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="P12" s="67">
+        <v>44646</v>
+      </c>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="79" t="s">
+        <v>89</v>
+      </c>
+      <c r="S12" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="T12" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="U12" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="V12" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="W12" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="X12" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y12" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z12" s="44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="29" customFormat="1">
+      <c r="A13" s="29">
+        <v>11</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="43">
+        <v>526258372598</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="44">
+        <v>1211</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="M13" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="N13" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="O13" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="P13" s="67">
+        <v>44646</v>
+      </c>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="80"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
+      <c r="X13" s="44"/>
+      <c r="Y13" s="44"/>
+      <c r="Z13" s="44"/>
+    </row>
+    <row r="14" spans="1:26" s="28" customFormat="1" ht="43.5">
+      <c r="A14" s="28">
+        <v>12</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="46">
+        <v>526251259145</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="41">
+        <v>1211</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="J14" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="P14" s="64">
+        <v>44646</v>
+      </c>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="S14" s="82" t="s">
+        <v>101</v>
+      </c>
+      <c r="T14" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="U14" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="V14" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="W14" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="X14" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y14" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z14" s="41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="29" customFormat="1">
+      <c r="A15" s="29">
+        <v>13</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="43">
+        <v>526251037317</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="45">
-        <v>526251020232</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="46" t="s">
+      <c r="E15" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F15" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="47">
+      <c r="G15" s="44">
         <v>1312</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H15" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="46" t="s">
+      <c r="I15" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="M15" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="N15" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="O15" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="P15" s="67">
+        <v>44646</v>
+      </c>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="83" t="s">
+        <v>110</v>
+      </c>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="44"/>
+      <c r="Y15" s="44"/>
+      <c r="Z15" s="44"/>
+    </row>
+    <row r="16" spans="1:26" s="28" customFormat="1" ht="48" customHeight="1">
+      <c r="A16" s="28">
+        <v>14</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="46">
+        <v>526251060168</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="41">
+        <v>1211</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="J16" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="70" t="s">
+      <c r="K16" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="M11" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="N11" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="O11" s="71" t="s">
-        <v>85</v>
-      </c>
-      <c r="P11" s="72">
-        <v>44646</v>
-      </c>
-      <c r="R11" s="87"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="47"/>
-      <c r="V11" s="47"/>
-      <c r="W11" s="47"/>
-      <c r="X11" s="47"/>
-      <c r="Y11" s="47"/>
-      <c r="Z11" s="47"/>
-    </row>
-    <row r="12" s="33" customFormat="1" spans="1:26">
-      <c r="A12" s="33">
-        <v>10</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="49">
-        <v>526251531996</v>
-      </c>
-      <c r="D12" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="50">
-        <v>1211</v>
-      </c>
-      <c r="H12" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="J12" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="73" t="s">
-        <v>82</v>
-      </c>
-      <c r="M12" s="73" t="s">
-        <v>88</v>
-      </c>
-      <c r="N12" s="73" t="s">
+      <c r="L16" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="N16" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="P12" s="75">
-        <v>44646</v>
-      </c>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="S12" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="T12" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="U12" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="V12" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="W12" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="X12" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y12" s="98" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z12" s="50" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" s="33" customFormat="1" spans="1:26">
-      <c r="A13" s="33">
-        <v>11</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="49">
-        <v>526258372598</v>
-      </c>
-      <c r="D13" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="50">
-        <v>1211</v>
-      </c>
-      <c r="H13" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="K13" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="73" t="s">
-        <v>82</v>
-      </c>
-      <c r="M13" s="73" t="s">
-        <v>95</v>
-      </c>
-      <c r="N13" s="73" t="s">
-        <v>84</v>
-      </c>
-      <c r="O13" s="74" t="s">
-        <v>96</v>
-      </c>
-      <c r="P13" s="75">
-        <v>44646</v>
-      </c>
-      <c r="Q13" s="73"/>
-      <c r="R13" s="89"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="50"/>
-      <c r="Z13" s="50"/>
-    </row>
-    <row r="14" s="32" customFormat="1" ht="45" spans="1:26">
-      <c r="A14" s="32">
-        <v>12</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="52">
-        <v>526251259145</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="47">
-        <v>1211</v>
-      </c>
-      <c r="H14" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="70" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="M14" s="70" t="s">
-        <v>99</v>
-      </c>
-      <c r="N14" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="O14" s="71" t="s">
-        <v>100</v>
-      </c>
-      <c r="P14" s="72">
-        <v>44646</v>
-      </c>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="91" t="s">
-        <v>101</v>
-      </c>
-      <c r="S14" s="92" t="s">
-        <v>102</v>
-      </c>
-      <c r="T14" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="U14" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="V14" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="W14" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="X14" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y14" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="Z14" s="46" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" s="33" customFormat="1" spans="1:26">
-      <c r="A15" s="33">
-        <v>13</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" s="49">
-        <v>526251037317</v>
-      </c>
-      <c r="D15" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="50">
-        <v>1312</v>
-      </c>
-      <c r="H15" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="I15" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="J15" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="73" t="s">
-        <v>82</v>
-      </c>
-      <c r="M15" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="N15" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="O15" s="74" t="s">
-        <v>110</v>
-      </c>
-      <c r="P15" s="75">
-        <v>44646</v>
-      </c>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="93" t="s">
-        <v>111</v>
-      </c>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
-      <c r="U15" s="50"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="50"/>
-      <c r="X15" s="50"/>
-      <c r="Y15" s="50"/>
-      <c r="Z15" s="50"/>
-    </row>
-    <row r="16" s="32" customFormat="1" ht="48" customHeight="1" spans="1:26">
-      <c r="A16" s="32">
-        <v>14</v>
-      </c>
-      <c r="B16" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="52">
-        <v>526251060168</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="47">
-        <v>1211</v>
-      </c>
-      <c r="H16" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="J16" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="70" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="M16" s="76" t="s">
+      <c r="O16" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="N16" s="76" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="77" t="s">
+      <c r="P16" s="64">
+        <v>44762</v>
+      </c>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="P16" s="72">
-        <v>44762</v>
-      </c>
-      <c r="Q16" s="90"/>
-      <c r="R16" s="94" t="s">
-        <v>116</v>
-      </c>
-      <c r="S16" s="47"/>
-      <c r="T16" s="47"/>
-      <c r="U16" s="47"/>
-      <c r="V16" s="47"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="47"/>
-      <c r="Y16" s="47"/>
-      <c r="Z16" s="47"/>
-    </row>
-    <row r="17" s="10" customFormat="1" spans="1:26">
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="41"/>
+      <c r="Z16" s="41"/>
+    </row>
+    <row r="17" spans="1:26" s="10" customFormat="1">
       <c r="A17" s="10">
         <v>15</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="16">
         <v>526251059200</v>
       </c>
       <c r="D17" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>118</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>119</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>21</v>
@@ -2885,31 +2245,31 @@
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="66" t="s">
+      <c r="K17" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="66" t="s">
+      <c r="L17" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="M17" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="M17" s="66" t="s">
+      <c r="N17" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="N17" s="66" t="s">
+      <c r="O17" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="O17" s="78" t="s">
-        <v>124</v>
-      </c>
-      <c r="P17" s="24">
+      <c r="P17" s="22">
         <v>44647</v>
       </c>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="95"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="85"/>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
       <c r="U17" s="17"/>
@@ -2919,14 +2279,14 @@
       <c r="Y17" s="17"/>
       <c r="Z17" s="17"/>
     </row>
-    <row r="18" s="10" customFormat="1" spans="1:26">
+    <row r="18" spans="1:26" s="10" customFormat="1">
       <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="B18" s="53" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" s="54">
+      <c r="B18" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="48">
         <v>526251020790</v>
       </c>
       <c r="D18" s="17" t="s">
@@ -2943,30 +2303,30 @@
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="66" t="s">
+      <c r="K18" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="66" t="s">
-        <v>121</v>
-      </c>
-      <c r="M18" s="66" t="s">
+      <c r="L18" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="M18" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="N18" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="O18" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="N18" s="66" t="s">
-        <v>123</v>
-      </c>
-      <c r="O18" s="78" t="s">
-        <v>128</v>
-      </c>
-      <c r="P18" s="24">
+      <c r="P18" s="22">
         <v>44647</v>
       </c>
-      <c r="R18" s="95"/>
+      <c r="R18" s="85"/>
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
       <c r="U18" s="17"/>
@@ -2976,47 +2336,47 @@
       <c r="Y18" s="17"/>
       <c r="Z18" s="17"/>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="55">
+    <row r="19" spans="1:26">
+      <c r="A19" s="49">
         <v>17</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="51">
+        <v>526251020642</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="31">
+        <v>1211</v>
+      </c>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31" t="s">
         <v>129</v>
-      </c>
-      <c r="C19" s="57">
-        <v>526251020642</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="36">
-        <v>1211</v>
-      </c>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36" t="s">
-        <v>130</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="79" t="s">
+      <c r="K19" s="70" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" s="34" customFormat="1" spans="1:26">
-      <c r="A20" s="34">
+    <row r="20" spans="1:26" s="11" customFormat="1">
+      <c r="A20" s="11">
         <v>19</v>
       </c>
-      <c r="B20" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="C20" s="59">
+      <c r="B20" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="53">
         <v>526251579804</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -3028,139 +2388,133 @@
       <c r="F20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="60">
+      <c r="G20" s="9">
         <v>1211</v>
       </c>
-      <c r="H20" s="60"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K20" s="80" t="s">
+      <c r="K20" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="96"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="60"/>
-      <c r="U20" s="60"/>
-      <c r="V20" s="60"/>
-      <c r="W20" s="60"/>
-      <c r="X20" s="60"/>
-      <c r="Y20" s="60"/>
-      <c r="Z20" s="60"/>
-    </row>
-    <row r="22" s="35" customFormat="1" spans="2:26">
-      <c r="B22" s="61" t="s">
+      <c r="O20" s="72"/>
+      <c r="P20" s="73"/>
+      <c r="R20" s="86"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+    </row>
+    <row r="22" spans="1:26" s="30" customFormat="1">
+      <c r="B22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="I22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="J22" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="K22" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="E22" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="G22" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="H22" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="I22" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="J22" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="K22" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="L22" s="35" t="s">
+      <c r="M22" s="89" t="s">
         <v>134</v>
       </c>
-      <c r="M22" s="99" t="s">
+      <c r="N22" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="O22" s="75" t="s">
         <v>135</v>
       </c>
-      <c r="N22" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="O22" s="84" t="s">
-        <v>136</v>
-      </c>
-      <c r="R22" s="97"/>
-      <c r="S22" s="61"/>
-      <c r="T22" s="61"/>
-      <c r="U22" s="61"/>
-      <c r="V22" s="61"/>
-      <c r="W22" s="61"/>
-      <c r="X22" s="61"/>
-      <c r="Y22" s="61"/>
-      <c r="Z22" s="61"/>
+      <c r="R22" s="87"/>
+      <c r="S22" s="54"/>
+      <c r="T22" s="54"/>
+      <c r="U22" s="54"/>
+      <c r="V22" s="54"/>
+      <c r="W22" s="54"/>
+      <c r="X22" s="54"/>
+      <c r="Y22" s="54"/>
+      <c r="Z22" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="R1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5428571428571" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.18095238095238" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.4571428571429" style="12" customWidth="1"/>
-    <col min="3" max="3" width="15.7238095238095" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.1809523809524" style="12" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="12" customWidth="1"/>
     <col min="5" max="5" width="10" style="12" customWidth="1"/>
-    <col min="6" max="6" width="6.81904761904762" style="12" customWidth="1"/>
-    <col min="7" max="7" width="24.5714285714286" style="12" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" style="12" customWidth="1"/>
     <col min="8" max="8" width="14" style="12" customWidth="1"/>
-    <col min="9" max="9" width="39.2666666666667" style="12" customWidth="1"/>
-    <col min="10" max="10" width="15.4571428571429" style="12" customWidth="1"/>
-    <col min="11" max="11" width="20.7142857142857" style="12" customWidth="1"/>
-    <col min="12" max="12" width="22.8571428571429" style="12" customWidth="1"/>
-    <col min="13" max="13" width="11.8666666666667" style="12" customWidth="1"/>
-    <col min="14" max="14" width="10.8857142857143" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.4380952380952" style="12" customWidth="1"/>
-    <col min="16" max="16" width="10.8857142857143" style="12" customWidth="1"/>
-    <col min="17" max="17" width="10.4380952380952" style="12" customWidth="1"/>
-    <col min="18" max="18" width="10.8857142857143" style="12" customWidth="1"/>
-    <col min="19" max="19" width="10.4380952380952" style="12" customWidth="1"/>
-    <col min="20" max="21" width="19.1809523809524" style="12" customWidth="1"/>
-    <col min="22" max="22" width="60.2666666666667" style="13" customWidth="1"/>
-    <col min="23" max="16384" width="11.5428571428571" style="12"/>
+    <col min="9" max="9" width="39.26953125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="20.7265625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="10.90625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" style="12" customWidth="1"/>
+    <col min="16" max="16" width="10.90625" style="12" customWidth="1"/>
+    <col min="17" max="17" width="10.453125" style="12" customWidth="1"/>
+    <col min="18" max="18" width="10.90625" style="12" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" style="12" customWidth="1"/>
+    <col min="20" max="21" width="19.1796875" style="12" customWidth="1"/>
+    <col min="22" max="22" width="60.26953125" style="13" customWidth="1"/>
+    <col min="23" max="16384" width="11.54296875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="22:22">
+    <row r="1" spans="1:30">
       <c r="V1" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="9" customFormat="1" spans="1:22">
+    <row r="2" spans="1:30" s="9" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -3198,25 +2552,25 @@
         <v>15</v>
       </c>
       <c r="M2" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>16</v>
@@ -3228,127 +2582,125 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="1" spans="1:22">
+    <row r="3" spans="1:30" s="10" customFormat="1">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>145</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="J3" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="L3" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="26">
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="24">
         <v>44603</v>
       </c>
       <c r="U3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" s="11" customFormat="1" spans="1:30">
+      <c r="V3" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" s="11" customFormat="1">
       <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="20">
         <v>526251020596</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="21" t="s">
+      <c r="H4" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="H4" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="L4" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="V4" s="28"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="29"/>
-      <c r="AD4" s="29"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" display="http://pprsar.com/cosme/commj_v2.php"/>
-    <hyperlink ref="I4" r:id="rId1" display="http://pprsar.com/cosme/commj_v2.php"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4571428571429" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.5428571428571" customWidth="1"/>
-    <col min="2" max="2" width="15.5428571428571" customWidth="1"/>
-    <col min="5" max="5" width="36.8190476190476" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="36.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3359,13 +2711,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3382,7 +2734,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3399,12 +2751,12 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="3">
         <v>526251531996</v>
@@ -3416,12 +2768,12 @@
         <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="6">
         <v>526258372598</v>
@@ -3433,12 +2785,12 @@
         <v>18</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="3">
         <v>526251059200</v>
@@ -3450,12 +2802,12 @@
         <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="6">
         <v>526251259145</v>
@@ -3467,7 +2819,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3484,7 +2836,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3501,7 +2853,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3518,12 +2870,12 @@
         <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="6">
         <v>526251060168</v>
@@ -3535,12 +2887,12 @@
         <v>18</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="3">
         <v>526251037317</v>
@@ -3552,7 +2904,7 @@
         <v>32</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3569,7 +2921,7 @@
         <v>32</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3586,12 +2938,12 @@
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B15" s="6">
         <v>526251579804</v>
@@ -3603,7 +2955,7 @@
         <v>32</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3620,12 +2972,12 @@
         <v>32</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" s="6">
         <v>526251020232</v>
@@ -3633,23 +2985,23 @@
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" s="3">
         <v>526251020790</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" s="6">
         <v>526251020642</v>
@@ -3657,22 +3009,21 @@
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" s="3">
         <v>526251020596</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mejoras en la interfaz de usuario
- Unificación de componentes en la PWA:
   . Ventanas
   . Tipografía
   . Estilos
   . Imágenes
   . Desplegables
</commit_message>
<xml_diff>
--- a/Documentación/Empresa/Control de equipos.xlsx
+++ b/Documentación/Empresa/Control de equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cosme\Documents\GitHub\dta-agricola\Documentación\Empresa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cosmesantiesteban/Documents/GitHub/dta-agricola/Documentación/Empresa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3245CEC5-7BEB-4814-A4CD-E53ABB0ECA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB2C599-A25E-7841-9D4D-D1FC09F6F915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="491" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="491" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movimiento contínuo" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="179">
   <si>
     <t>Observaciones</t>
   </si>
@@ -565,7 +565,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,7 +592,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -600,7 +600,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -608,7 +608,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -616,26 +616,27 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -726,20 +727,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -752,7 +739,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,6 +794,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -832,7 +825,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1145,50 +1138,36 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1201,10 +1180,23 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1487,43 +1479,43 @@
       <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="12" customWidth="1"/>
     <col min="5" max="5" width="10" style="12" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="7.54296875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="31.26953125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="19.453125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="37.81640625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" style="12" customWidth="1"/>
-    <col min="13" max="13" width="20.26953125" style="12" customWidth="1"/>
-    <col min="14" max="14" width="10.81640625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="26.1796875" style="12" customWidth="1"/>
-    <col min="16" max="17" width="19.1796875" style="12" customWidth="1"/>
-    <col min="18" max="18" width="60.26953125" style="13" customWidth="1"/>
-    <col min="19" max="26" width="12.1796875" style="30" customWidth="1"/>
-    <col min="27" max="16384" width="11.54296875" style="12"/>
+    <col min="6" max="6" width="6.83203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="7.5" style="12" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="12" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="12" customWidth="1"/>
+    <col min="11" max="11" width="37.83203125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="12" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="12" customWidth="1"/>
+    <col min="15" max="15" width="26.1640625" style="12" customWidth="1"/>
+    <col min="16" max="17" width="19.1640625" style="12" customWidth="1"/>
+    <col min="18" max="18" width="60.33203125" style="13" customWidth="1"/>
+    <col min="19" max="26" width="12.1640625" style="30" customWidth="1"/>
+    <col min="27" max="16384" width="11.5" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="R1" s="112" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
-      <c r="Z1" s="112"/>
-    </row>
-    <row r="2" spans="1:26" s="9" customFormat="1">
+      <c r="S1" s="125"/>
+      <c r="T1" s="125"/>
+      <c r="U1" s="125"/>
+      <c r="V1" s="125"/>
+      <c r="W1" s="125"/>
+      <c r="X1" s="125"/>
+      <c r="Y1" s="125"/>
+      <c r="Z1" s="125"/>
+    </row>
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1603,7 +1595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="11" customFormat="1">
+    <row r="3" spans="1:26" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
         <v>1</v>
       </c>
@@ -1663,7 +1655,7 @@
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
     </row>
-    <row r="4" spans="1:26" s="82" customFormat="1" ht="29">
+    <row r="4" spans="1:26" s="82" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="82">
         <v>2</v>
       </c>
@@ -1725,7 +1717,7 @@
       <c r="Y4" s="81"/>
       <c r="Z4" s="81"/>
     </row>
-    <row r="5" spans="1:26" s="82" customFormat="1" ht="29">
+    <row r="5" spans="1:26" s="82" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="82">
         <v>3</v>
       </c>
@@ -1787,7 +1779,7 @@
       <c r="Y5" s="81"/>
       <c r="Z5" s="81"/>
     </row>
-    <row r="6" spans="1:26" s="82" customFormat="1">
+    <row r="6" spans="1:26" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="82">
         <v>4</v>
       </c>
@@ -1849,7 +1841,7 @@
       <c r="Y6" s="81"/>
       <c r="Z6" s="81"/>
     </row>
-    <row r="7" spans="1:26" s="82" customFormat="1">
+    <row r="7" spans="1:26" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="82">
         <v>5</v>
       </c>
@@ -1911,7 +1903,7 @@
       <c r="Y7" s="81"/>
       <c r="Z7" s="81"/>
     </row>
-    <row r="8" spans="1:26" s="82" customFormat="1">
+    <row r="8" spans="1:26" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="82">
         <v>6</v>
       </c>
@@ -1973,7 +1965,7 @@
       <c r="Y8" s="81"/>
       <c r="Z8" s="81"/>
     </row>
-    <row r="9" spans="1:26" s="82" customFormat="1">
+    <row r="9" spans="1:26" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="82">
         <v>7</v>
       </c>
@@ -2029,7 +2021,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="27" customFormat="1">
+    <row r="10" spans="1:26" s="27" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
         <v>8</v>
       </c>
@@ -2090,7 +2082,7 @@
       <c r="Y10" s="37"/>
       <c r="Z10" s="37"/>
     </row>
-    <row r="11" spans="1:26" s="28" customFormat="1">
+    <row r="11" spans="1:26" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="61">
         <v>9</v>
       </c>
@@ -2150,7 +2142,7 @@
       <c r="Y11" s="59"/>
       <c r="Z11" s="59"/>
     </row>
-    <row r="12" spans="1:26" s="82" customFormat="1">
+    <row r="12" spans="1:26" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="82">
         <v>10</v>
       </c>
@@ -2228,7 +2220,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="82" customFormat="1">
+    <row r="13" spans="1:26" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="82">
         <v>11</v>
       </c>
@@ -2288,7 +2280,7 @@
       <c r="Y13" s="81"/>
       <c r="Z13" s="81"/>
     </row>
-    <row r="14" spans="1:26" s="28" customFormat="1" ht="43.5">
+    <row r="14" spans="1:26" s="28" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="61">
         <v>12</v>
       </c>
@@ -2366,7 +2358,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="94" customFormat="1">
+    <row r="15" spans="1:26" s="94" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="94">
         <v>13</v>
       </c>
@@ -2428,7 +2420,7 @@
       <c r="Y15" s="97"/>
       <c r="Z15" s="97"/>
     </row>
-    <row r="16" spans="1:26" s="28" customFormat="1" ht="48" customHeight="1">
+    <row r="16" spans="1:26" s="28" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="57">
         <v>14</v>
       </c>
@@ -2490,7 +2482,7 @@
       <c r="Y16" s="59"/>
       <c r="Z16" s="59"/>
     </row>
-    <row r="17" spans="1:26" s="94" customFormat="1">
+    <row r="17" spans="1:26" s="94" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="94">
         <v>15</v>
       </c>
@@ -2548,7 +2540,7 @@
       <c r="Y17" s="97"/>
       <c r="Z17" s="97"/>
     </row>
-    <row r="18" spans="1:26" s="82" customFormat="1">
+    <row r="18" spans="1:26" s="82" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="82">
         <v>16</v>
       </c>
@@ -2605,7 +2597,7 @@
       <c r="Y18" s="81"/>
       <c r="Z18" s="81"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="61">
         <v>17</v>
       </c>
@@ -2653,7 +2645,7 @@
       <c r="Y19" s="59"/>
       <c r="Z19" s="59"/>
     </row>
-    <row r="20" spans="1:26" s="11" customFormat="1">
+    <row r="20" spans="1:26" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="65">
         <v>19</v>
       </c>
@@ -2701,10 +2693,10 @@
       <c r="Y20" s="68"/>
       <c r="Z20" s="68"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="J21" s="90"/>
     </row>
-    <row r="22" spans="1:26" s="29" customFormat="1">
+    <row r="22" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="38" t="s">
         <v>131</v>
       </c>
@@ -2774,38 +2766,38 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="12" customWidth="1"/>
     <col min="5" max="5" width="10" style="12" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="24.54296875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="12" customWidth="1"/>
     <col min="8" max="8" width="14" style="12" customWidth="1"/>
-    <col min="9" max="9" width="39.26953125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="20.7265625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="22.81640625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" style="12" customWidth="1"/>
-    <col min="14" max="14" width="10.90625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="10.90625" style="12" customWidth="1"/>
-    <col min="17" max="17" width="10.453125" style="12" customWidth="1"/>
-    <col min="18" max="18" width="10.90625" style="12" customWidth="1"/>
-    <col min="19" max="19" width="10.453125" style="12" customWidth="1"/>
-    <col min="20" max="21" width="19.1796875" style="12" customWidth="1"/>
-    <col min="22" max="22" width="60.26953125" style="13" customWidth="1"/>
-    <col min="23" max="16384" width="11.54296875" style="12"/>
+    <col min="9" max="9" width="39.33203125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="12" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="12" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="12" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="12" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="12" customWidth="1"/>
+    <col min="19" max="19" width="10.5" style="12" customWidth="1"/>
+    <col min="20" max="21" width="19.1640625" style="12" customWidth="1"/>
+    <col min="22" max="22" width="60.33203125" style="13" customWidth="1"/>
+    <col min="23" max="16384" width="11.5" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="V1" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="9" customFormat="1">
+    <row r="2" spans="1:30" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -2873,7 +2865,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="10" customFormat="1">
+    <row r="3" spans="1:30" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -2923,7 +2915,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="11" customFormat="1">
+    <row r="4" spans="1:30" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -2970,7 +2962,7 @@
       <c r="AC4" s="9"/>
       <c r="AD4" s="9"/>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="56">
         <v>3</v>
       </c>
@@ -3024,20 +3016,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="36.81640625" customWidth="1"/>
-    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3054,62 +3046,62 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="130" customFormat="1">
-      <c r="A2" s="130" t="s">
+    <row r="2" spans="1:10" s="124" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="130">
+      <c r="B2" s="119">
         <v>526251106286</v>
       </c>
-      <c r="C2" s="130">
+      <c r="C2" s="124">
         <v>32845128</v>
       </c>
-      <c r="D2" s="130">
+      <c r="D2" s="124">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="124" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="130" t="s">
+      <c r="G2" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="130" t="s">
+      <c r="H2" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="124" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="130" t="s">
+      <c r="J2" s="124" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="116" customFormat="1">
-      <c r="A3" s="113" t="s">
+    <row r="3" spans="1:10" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="114">
+      <c r="B3" s="108">
         <v>526251024489</v>
       </c>
-      <c r="C3" s="115">
+      <c r="C3" s="109">
         <v>32845129</v>
       </c>
-      <c r="D3" s="115">
+      <c r="D3" s="109">
         <v>18</v>
       </c>
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="G3" s="116" t="s">
+      <c r="G3" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="116" t="s">
+      <c r="H3" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I3" s="116" t="s">
+      <c r="I3" s="110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>85</v>
       </c>
@@ -3125,60 +3117,63 @@
       <c r="E4" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="107" t="s">
+      <c r="G4" s="106" t="s">
         <v>87</v>
       </c>
       <c r="H4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="116" customFormat="1">
-      <c r="A5" s="113" t="s">
+    <row r="5" spans="1:10" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="107" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="114">
+      <c r="B5" s="108">
         <v>526258372598</v>
       </c>
-      <c r="C5" s="115">
+      <c r="C5" s="109">
         <v>32845131</v>
       </c>
-      <c r="D5" s="115">
+      <c r="D5" s="109">
         <v>18</v>
       </c>
-      <c r="E5" s="115" t="s">
+      <c r="E5" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="116" t="s">
+      <c r="G5" s="110" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="116" t="s">
+      <c r="H5" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I5" s="116" t="s">
+      <c r="I5" s="110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="111" customFormat="1">
-      <c r="A6" s="108" t="s">
+    <row r="6" spans="1:10" s="129" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="126" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="109">
+      <c r="B6" s="127">
         <v>526251059200</v>
       </c>
-      <c r="C6" s="110">
+      <c r="C6" s="128">
         <v>32845132</v>
       </c>
-      <c r="D6" s="110">
+      <c r="D6" s="128">
         <v>18</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="128" t="s">
         <v>158</v>
       </c>
-      <c r="G6" s="111" t="s">
+      <c r="G6" s="129" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6" s="129" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>95</v>
       </c>
@@ -3194,92 +3189,92 @@
       <c r="E7" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="107" t="s">
+      <c r="G7" s="106" t="s">
         <v>97</v>
       </c>
       <c r="H7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="116" customFormat="1">
-      <c r="A8" s="117" t="s">
+    <row r="8" spans="1:10" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="118">
+      <c r="B8" s="112">
         <v>526255917395</v>
       </c>
-      <c r="C8" s="119">
+      <c r="C8" s="113">
         <v>32845135</v>
       </c>
-      <c r="D8" s="119">
+      <c r="D8" s="113">
         <v>18</v>
       </c>
-      <c r="E8" s="119" t="s">
+      <c r="E8" s="113" t="s">
         <v>158</v>
       </c>
-      <c r="G8" s="116" t="s">
+      <c r="G8" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="116" t="s">
+      <c r="H8" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I8" s="116" t="s">
+      <c r="I8" s="110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="116" customFormat="1">
-      <c r="A9" s="113" t="s">
+    <row r="9" spans="1:10" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="114">
+      <c r="B9" s="108">
         <v>526251271378</v>
       </c>
-      <c r="C9" s="115">
+      <c r="C9" s="109">
         <v>32848029</v>
       </c>
-      <c r="D9" s="115">
+      <c r="D9" s="109">
         <v>18</v>
       </c>
-      <c r="E9" s="115" t="s">
+      <c r="E9" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="G9" s="116" t="s">
+      <c r="G9" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="116" t="s">
+      <c r="H9" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I9" s="116" t="s">
+      <c r="I9" s="110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="116" customFormat="1">
-      <c r="A10" s="117" t="s">
+    <row r="10" spans="1:10" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="118">
+      <c r="B10" s="112">
         <v>526251193016</v>
       </c>
-      <c r="C10" s="119">
+      <c r="C10" s="113">
         <v>32848031</v>
       </c>
-      <c r="D10" s="119">
+      <c r="D10" s="113">
         <v>18</v>
       </c>
-      <c r="E10" s="119" t="s">
+      <c r="E10" s="113" t="s">
         <v>158</v>
       </c>
-      <c r="G10" s="116" t="s">
+      <c r="G10" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="116" t="s">
+      <c r="H10" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I10" s="116" t="s">
+      <c r="I10" s="110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>110</v>
       </c>
@@ -3295,86 +3290,89 @@
       <c r="E11" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G11" s="107" t="s">
+      <c r="G11" s="106" t="s">
         <v>175</v>
       </c>
       <c r="H11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="111" customFormat="1">
-      <c r="A12" s="108" t="s">
+    <row r="12" spans="1:10" s="129" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="126" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="109">
+      <c r="B12" s="127">
         <v>526251037317</v>
       </c>
-      <c r="C12" s="110">
+      <c r="C12" s="128">
         <v>32848094</v>
       </c>
-      <c r="D12" s="110">
+      <c r="D12" s="128">
         <v>32</v>
       </c>
-      <c r="E12" s="110" t="s">
+      <c r="E12" s="128" t="s">
         <v>158</v>
       </c>
-      <c r="G12" s="111" t="s">
+      <c r="G12" s="129" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="116" customFormat="1">
-      <c r="A13" s="113" t="s">
+      <c r="J12" s="129" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="114">
+      <c r="B13" s="108">
         <v>526251452797</v>
       </c>
-      <c r="C13" s="115">
+      <c r="C13" s="109">
         <v>32848096</v>
       </c>
-      <c r="D13" s="115">
+      <c r="D13" s="109">
         <v>32</v>
       </c>
-      <c r="E13" s="115" t="s">
+      <c r="E13" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="G13" s="116" t="s">
+      <c r="G13" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="116" t="s">
+      <c r="H13" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I13" s="116" t="s">
+      <c r="I13" s="110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="127" customFormat="1">
-      <c r="A14" s="124" t="s">
+    <row r="14" spans="1:10" s="121" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="125">
+      <c r="B14" s="119">
         <v>526251342314</v>
       </c>
-      <c r="C14" s="126">
+      <c r="C14" s="120">
         <v>32848097</v>
       </c>
-      <c r="D14" s="126">
+      <c r="D14" s="120">
         <v>32</v>
       </c>
-      <c r="E14" s="126" t="s">
+      <c r="E14" s="120" t="s">
         <v>158</v>
       </c>
-      <c r="G14" s="128" t="s">
+      <c r="G14" s="122" t="s">
         <v>170</v>
       </c>
-      <c r="H14" s="127" t="s">
+      <c r="H14" s="121" t="s">
         <v>174</v>
       </c>
-      <c r="J14" s="129" t="s">
+      <c r="J14" s="123" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>129</v>
       </c>
@@ -3397,50 +3395,53 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="116" customFormat="1">
-      <c r="A16" s="120" t="s">
+    <row r="16" spans="1:10" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="121">
+      <c r="B16" s="115">
         <v>526251201079</v>
       </c>
-      <c r="C16" s="122">
+      <c r="C16" s="116">
         <v>32848099</v>
       </c>
-      <c r="D16" s="122">
+      <c r="D16" s="116">
         <v>32</v>
       </c>
-      <c r="E16" s="122" t="s">
+      <c r="E16" s="116" t="s">
         <v>158</v>
       </c>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123" t="s">
+      <c r="F16" s="117"/>
+      <c r="G16" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="H16" s="123" t="s">
+      <c r="H16" s="117" t="s">
         <v>173</v>
       </c>
-      <c r="I16" s="116" t="s">
+      <c r="I16" s="110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:10" s="129" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="127">
         <v>526251020232</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="7" t="s">
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="128" t="s">
         <v>158</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="129" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="J17" s="129" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3450,14 +3451,14 @@
       <c r="E18" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G18" s="107" t="s">
+      <c r="G18" s="106" t="s">
         <v>125</v>
       </c>
       <c r="H18" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>127</v>
       </c>
@@ -3476,46 +3477,46 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="116" customFormat="1">
-      <c r="A20" s="116" t="s">
+    <row r="20" spans="1:10" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="110" t="s">
         <v>151</v>
       </c>
-      <c r="B20" s="118">
+      <c r="B20" s="112">
         <v>526251020596</v>
       </c>
-      <c r="E20" s="119" t="s">
+      <c r="E20" s="113" t="s">
         <v>158</v>
       </c>
-      <c r="G20" s="116" t="s">
+      <c r="G20" s="110" t="s">
         <v>152</v>
       </c>
-      <c r="H20" s="116" t="s">
+      <c r="H20" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I20" s="116" t="s">
+      <c r="I20" s="110" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="130" customFormat="1">
-      <c r="A21" s="130" t="s">
+    <row r="21" spans="1:10" s="124" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="124" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="130">
+      <c r="B21" s="119">
         <v>526251020266</v>
       </c>
-      <c r="E21" s="130" t="s">
+      <c r="E21" s="124" t="s">
         <v>158</v>
       </c>
-      <c r="G21" s="130" t="s">
+      <c r="G21" s="124" t="s">
         <v>172</v>
       </c>
-      <c r="H21" s="130" t="s">
+      <c r="H21" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="I21" s="130" t="s">
+      <c r="I21" s="124" t="s">
         <v>177</v>
       </c>
-      <c r="J21" s="130" t="s">
+      <c r="J21" s="124" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DTA - Protocolo de calibración SHT4x
</commit_message>
<xml_diff>
--- a/Documentación/Empresa/Control de equipos.xlsx
+++ b/Documentación/Empresa/Control de equipos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DTA-Agrícola\Documents\GitHub\dta-agricola\Documentación\Empresa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AC53E4-59D8-4EED-B785-631633911766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2D4CD6-4F2C-453E-B0EE-C29F71FF93DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="577" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6705" yWindow="2655" windowWidth="20730" windowHeight="11160" tabRatio="577" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movimiento contínuo" sheetId="8" r:id="rId1"/>
@@ -1531,11 +1531,11 @@
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1846,17 +1846,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="R1" s="170" t="s">
+      <c r="R1" s="171" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="170"/>
-      <c r="T1" s="170"/>
-      <c r="U1" s="170"/>
-      <c r="V1" s="170"/>
-      <c r="W1" s="170"/>
-      <c r="X1" s="170"/>
-      <c r="Y1" s="170"/>
-      <c r="Z1" s="170"/>
+      <c r="S1" s="171"/>
+      <c r="T1" s="171"/>
+      <c r="U1" s="171"/>
+      <c r="V1" s="171"/>
+      <c r="W1" s="171"/>
+      <c r="X1" s="171"/>
+      <c r="Y1" s="171"/>
+      <c r="Z1" s="171"/>
     </row>
     <row r="2" spans="1:26" s="37" customFormat="1">
       <c r="A2" s="37" t="s">
@@ -3414,10 +3414,10 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3535,7 +3535,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="19" customFormat="1" ht="14.1" customHeight="1">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="170" t="s">
         <v>236</v>
       </c>
       <c r="B4" s="35">
@@ -3609,10 +3609,10 @@
       </c>
       <c r="H8" s="163"/>
       <c r="I8" s="160" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -3691,10 +3691,10 @@
       </c>
       <c r="H12" s="163"/>
       <c r="I12" s="160" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="J12">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:14">

</xml_diff>